<commit_message>
Updated Kevin hour log
</commit_message>
<xml_diff>
--- a/Work_Log/Kevin_Hours_Log.xlsx
+++ b/Work_Log/Kevin_Hours_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\K_Documents\CEN4908C\Senior_Design_TI_Project\Work_Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D7D15A-4B03-4A39-B285-C3D7DFAA563F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479C94F-2D42-45A2-B89A-EA5B4D6B0C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="-3690" windowWidth="19410" windowHeight="20985" xr2:uid="{1E1DE2E1-E43F-4C7B-805F-E7F882405594}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{1E1DE2E1-E43F-4C7B-805F-E7F882405594}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Kevin Su Senior Design Work Log</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Added and wired FTDI- USB to SPI converter and FTDI EEPROM.</t>
+  </si>
+  <si>
+    <t>Completed drawing IWRL6432AOP and wired it in the schematic along with an clock oscillator and power sources.</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5815A0D-EF96-486C-AACC-708D8CEA56AE}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,6 +523,7 @@
     <col min="1" max="1" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -827,6 +831,26 @@
         <v>19</v>
       </c>
     </row>
+    <row r="17" spans="2:7" ht="64" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45682</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>